<commit_message>
Adding Custom training code
</commit_message>
<xml_diff>
--- a/Datasets/Generated_GPT3_paper.xlsx
+++ b/Datasets/Generated_GPT3_paper.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://technionmail-my.sharepoint.com/personal/noam_kasten_campus_technion_ac_il/Documents/GoodNotes/Semester 8/Deep Learning/project/Dataset/4 models/PapersData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://technionmail-my.sharepoint.com/personal/noam_kasten_campus_technion_ac_il/Documents/GoodNotes/Semester 8/Deep Learning/project/code/HumanOrGPT/Datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="20" documentId="11_08AE610ABED24DA3C1A1FD4637D80896F98EED1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2094CE24-5BF3-4533-9349-C774B41EF419}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="14400" windowHeight="7350" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="גיליון1" sheetId="2" r:id="rId1"/>
@@ -4130,10 +4130,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4336,9 +4332,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5864E02-41B3-41B7-9B21-5BFEE5A25E01}">
   <dimension ref="A1:B974"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A954" workbookViewId="0">
-      <selection sqref="A1:B974"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>

</xml_diff>